<commit_message>
minor updates in license sheet
</commit_message>
<xml_diff>
--- a/SASPACer/addcnt/simple_example.xlsx
+++ b/SASPACer/addcnt/simple_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\SAS_PACKAGES\packages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mytakeda-my.sharepoint.com/personal/ryou_nakaya_takeda_com/Documents/仲家/SAS/SASPACer/SASPACer/addcnt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4C7A4D-0BA5-4C88-810E-2761C82B380C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{FF4C7A4D-0BA5-4C88-810E-2761C82B380C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B333D96-2AA7-43F4-A6F3-B5287DBB3504}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="863" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="863" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="description" sheetId="1" r:id="rId1"/>
@@ -85,25 +85,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">	Copyright (c) [YEAR] [Owner Name]
-  Permission is hereby granted, free of charge, to any person obtaining a copy  
-  of this software and associated documentation files (the "Software"), to deal 
-  in the Software without restriction, including without limitation the rights  
-  to use, copy, modify, merge, publish, distribute, sublicense, and/or sell     
-  copies of the Software, and to permit persons to whom the Software is         
-  furnished to do so, subject to the following conditions:                      
-  The above copyright notice and this permission notice shall be included       
-  in all copies or substantial portions of the Software.                        
-  THE SOFTWARE IS PROVIDED "AS IS", WITHOUT WARRANTY OF ANY KIND, EXPRESS OR    
-  IMPLIED, INCLUDING BUT NOT LIMITED TO THE WARRANTIES OF MERCHANTABILITY,      
-  FITNESS FOR A PARTICULAR PURPOSE AND NONINFRINGEMENT. IN NO EVENT SHALL THE   
-  AUTHORS OR COPYRIGHT HOLDERS BE LIABLE FOR ANY CLAIM, DAMAGES OR OTHER        
-  LIABILITY, WHETHER IN AN ACTION OF CONTRACT, TORT OR OTHERWISE, ARISING FROM, 
-  OUT OF OR IN CONNECTION WITH THE SOFTWARE OR THE USE OR OTHER DEALINGS IN THE 
-  SOFTWARE. </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>help</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -167,6 +148,25 @@
   <si>
     <t>This is macro to say hello to something.
 (e.g. %myhello2(obj=Taro))</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">	Copyright (c) [YEAR] [Owner Name]
+Permission is hereby granted, free of charge, to any person obtaining a copy  
+of this software and associated documentation files (the "Software"), to deal 
+in the Software without restriction, including without limitation the rights  
+to use, copy, modify, merge, publish, distribute, sublicense, and/or sell     
+copies of the Software, and to permit persons to whom the Software is         
+furnished to do so, subject to the following conditions:                      
+The above copyright notice and this permission notice shall be included       
+in all copies or substantial portions of the Software.                        
+THE SOFTWARE IS PROVIDED "AS IS", WITHOUT WARRANTY OF ANY KIND, EXPRESS OR    
+IMPLIED, INCLUDING BUT NOT LIMITED TO THE WARRANTIES OF MERCHANTABILITY,      
+FITNESS FOR A PARTICULAR PURPOSE AND NONINFRINGEMENT. IN NO EVENT SHALL THE   
+AUTHORS OR COPYRIGHT HOLDERS BE LIABLE FOR ANY CLAIM, DAMAGES OR OTHER         
+LIABILITY, WHETHER IN AN ACTION OF CONTRACT, TORT OR OTHERWISE, ARISING FROM, 
+OUT OF OR IN CONNECTION WITH THE SOFTWARE OR THE USE OR OTHER DEALINGS IN THE 
+SOFTWARE. </t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -563,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -571,7 +571,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -587,7 +587,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -595,7 +595,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -624,7 +624,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="6"/>
     </row>
@@ -633,7 +633,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -646,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA4723A-BC3E-47B2-B1DD-0A431AEFC984}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -660,7 +660,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -673,7 +673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2407937D-6862-4C42-A8B5-594F375883D2}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
@@ -687,39 +687,39 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="54" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" ht="54" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="6"/>
     </row>

</xml_diff>

<commit_message>
minor updates to license sheet
</commit_message>
<xml_diff>
--- a/SASPACer/addcnt/simple_example.xlsx
+++ b/SASPACer/addcnt/simple_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mytakeda-my.sharepoint.com/personal/ryou_nakaya_takeda_com/Documents/仲家/SAS/SASPACer/SASPACer/addcnt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{FF4C7A4D-0BA5-4C88-810E-2761C82B380C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B333D96-2AA7-43F4-A6F3-B5287DBB3504}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{FF4C7A4D-0BA5-4C88-810E-2761C82B380C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B5E92E9-63DE-4478-83DC-8DFDAD163CDD}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="863" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -152,18 +152,18 @@
   </si>
   <si>
     <t xml:space="preserve">	Copyright (c) [YEAR] [Owner Name]
-Permission is hereby granted, free of charge, to any person obtaining a copy  
-of this software and associated documentation files (the "Software"), to deal 
-in the Software without restriction, including without limitation the rights  
-to use, copy, modify, merge, publish, distribute, sublicense, and/or sell     
-copies of the Software, and to permit persons to whom the Software is         
+Permission is hereby granted, free of charge, to any person obtaining a copy   
+of this software and associated documentation files (the "Software"), to deal    
+in the Software without restriction, including without limitation the rights   
+to use, copy, modify, merge, publish, distribute, sublicense, and/or sell   
+copies of the Software, and to permit persons to whom the Software is   
 furnished to do so, subject to the following conditions:                      
 The above copyright notice and this permission notice shall be included       
 in all copies or substantial portions of the Software.                        
 THE SOFTWARE IS PROVIDED "AS IS", WITHOUT WARRANTY OF ANY KIND, EXPRESS OR    
 IMPLIED, INCLUDING BUT NOT LIMITED TO THE WARRANTIES OF MERCHANTABILITY,      
 FITNESS FOR A PARTICULAR PURPOSE AND NONINFRINGEMENT. IN NO EVENT SHALL THE   
-AUTHORS OR COPYRIGHT HOLDERS BE LIABLE FOR ANY CLAIM, DAMAGES OR OTHER         
+AUTHORS OR COPYRIGHT HOLDERS BE LIABLE FOR ANY CLAIM, DAMAGES OR OTHER        
 LIABILITY, WHETHER IN AN ACTION OF CONTRACT, TORT OR OTHERWISE, ARISING FROM, 
 OUT OF OR IN CONNECTION WITH THE SOFTWARE OR THE USE OR OTHER DEALINGS IN THE 
 SOFTWARE. </t>
@@ -647,7 +647,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>